<commit_message>
Corrected wealth codes & other
</commit_message>
<xml_diff>
--- a/data-input/country-codes/country-codes.xlsx
+++ b/data-input/country-codes/country-codes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iLucas/Dropbox/WID/Population/WorldNationalAccounts/stata-programs/country-codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasblanchet/GitHub/wid-world/data-input/country-codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="1100">
   <si>
     <t>code</t>
   </si>
@@ -3321,6 +3321,12 @@
   </si>
   <si>
     <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Middle East</t>
+  </si>
+  <si>
+    <t>the Middle East</t>
   </si>
 </sst>
 </file>
@@ -3678,8 +3684,8 @@
   <dimension ref="A1:F730"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E690" sqref="E690"/>
+      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C619" sqref="C619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9956,82 +9962,88 @@
         <v>988</v>
       </c>
     </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A609" s="1" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A611" s="1" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="612" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A612" s="1" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B612" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C612" s="2" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A613" s="1" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A614" s="1" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A615" s="1" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A616" s="1" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A617" s="1" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A619" s="1" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="620" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="621" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A621" s="1" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A623" s="1" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="624" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
         <v>865</v>
       </c>

</xml_diff>

<commit_message>
Included Middle East as a region
</commit_message>
<xml_diff>
--- a/data-input/country-codes/country-codes.xlsx
+++ b/data-input/country-codes/country-codes.xlsx
@@ -3352,6 +3352,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Courier"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3684,8 +3685,8 @@
   <dimension ref="A1:F730"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C619" sqref="C619"/>
+      <pane ySplit="1" topLeftCell="A597" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C613" sqref="C613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9982,10 +9983,10 @@
         <v>853</v>
       </c>
       <c r="B612" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C612" s="2" t="s">
         <v>1098</v>
-      </c>
-      <c r="C612" s="2" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update data quality + Organize project
</commit_message>
<xml_diff>
--- a/data-input/country-codes/country-codes.xlsx
+++ b/data-input/country-codes/country-codes.xlsx
@@ -3803,8 +3803,8 @@
   <dimension ref="A1:F744"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A283" sqref="A283"/>
+      <pane ySplit="1" topLeftCell="A518" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D523" sqref="D523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4515,10 +4515,10 @@
         <v>104</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -8713,10 +8713,10 @@
         <v>661</v>
       </c>
       <c r="D464" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E464" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="465" spans="1:6" x14ac:dyDescent="0.35">
@@ -9080,10 +9080,10 @@
         <v>961</v>
       </c>
       <c r="D490" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E490" s="6" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F490" s="6"/>
     </row>
@@ -9481,10 +9481,10 @@
         <v>754</v>
       </c>
       <c r="D522" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E522" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>